<commit_message>
update default max employee and tables under plots
</commit_message>
<xml_diff>
--- a/data/staffing_normal2020-04-08_other_additional input.xlsx
+++ b/data/staffing_normal2020-04-08_other_additional input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xilinchen/Documents/Repo/staff_projection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA68213-EFF3-F54B-9BC0-78EDF9A56DFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C9E651-FEE8-8A4D-948F-F78A4F892DEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,7 +600,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -611,7 +611,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -969,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1121,7 @@
         <v>0.74</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N4:N12" si="3">L4-(L4*M4)</f>
+        <f t="shared" ref="N4:N10" si="3">L4-(L4*M4)</f>
         <v>78</v>
       </c>
       <c r="O4" s="2">
@@ -1161,15 +1160,15 @@
         <f t="shared" si="2"/>
         <v>81.900000000000006</v>
       </c>
-      <c r="L5" s="6">
-        <v>300</v>
+      <c r="L5" s="3">
+        <v>200</v>
       </c>
       <c r="M5">
         <v>0.74</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="O5" s="2"/>
     </row>
@@ -1204,15 +1203,15 @@
         <f t="shared" si="2"/>
         <v>46.800000000000004</v>
       </c>
-      <c r="L6" s="6">
-        <v>300</v>
+      <c r="L6" s="3">
+        <v>100</v>
       </c>
       <c r="M6">
         <v>0.74</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="O6" s="2"/>
     </row>
@@ -1247,15 +1246,15 @@
         <f t="shared" si="2"/>
         <v>72.8</v>
       </c>
-      <c r="L7" s="6">
-        <v>300</v>
+      <c r="L7" s="3">
+        <v>100</v>
       </c>
       <c r="M7">
         <v>0.74</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="O7" s="2"/>
     </row>
@@ -1290,15 +1289,15 @@
         <f t="shared" si="2"/>
         <v>27.3</v>
       </c>
-      <c r="L8" s="6">
-        <v>300</v>
+      <c r="L8" s="3">
+        <v>50</v>
       </c>
       <c r="M8">
         <v>0.74</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="O8" s="2"/>
     </row>
@@ -1333,15 +1332,15 @@
         <f t="shared" si="2"/>
         <v>36.4</v>
       </c>
-      <c r="L9" s="6">
-        <v>300</v>
+      <c r="L9" s="3">
+        <v>50</v>
       </c>
       <c r="M9">
         <v>0.74</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="O9" s="2"/>
     </row>
@@ -1376,15 +1375,15 @@
         <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
-      <c r="L10" s="6">
-        <v>300</v>
+      <c r="L10" s="3">
+        <v>50</v>
       </c>
       <c r="M10">
         <v>0.74</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="O10" s="2"/>
     </row>
@@ -1419,15 +1418,15 @@
         <f t="shared" si="2"/>
         <v>20.8</v>
       </c>
-      <c r="L11" s="6">
-        <v>300</v>
+      <c r="L11" s="3">
+        <v>50</v>
       </c>
       <c r="M11">
         <v>0.74</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="3"/>
-        <v>78</v>
+        <f>L11-(L11*M11)</f>
+        <v>13</v>
       </c>
       <c r="O11" s="2"/>
     </row>
@@ -1462,17 +1461,20 @@
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="L12" s="6">
-        <v>300</v>
+      <c r="L12" s="3">
+        <v>50</v>
       </c>
       <c r="M12">
         <v>0.74</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="3"/>
-        <v>78</v>
+        <f>L12-(L12*M12)</f>
+        <v>13</v>
       </c>
       <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L13" s="3"/>
     </row>
     <row r="18" spans="7:8" ht="192" x14ac:dyDescent="0.2">
       <c r="G18" s="1" t="s">

</xml_diff>